<commit_message>
Modified accounts in sample Spreadsheet for Import of Accounts
</commit_message>
<xml_diff>
--- a/gkwebapp/static/spreadsheets/Account_Import_Spreadsheet.xlsx
+++ b/gkwebapp/static/spreadsheets/Account_Import_Spreadsheet.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t xml:space="preserve">Debit</t>
   </si>
@@ -31,10 +31,10 @@
     <t xml:space="preserve">Capital</t>
   </si>
   <si>
-    <t xml:space="preserve">abcd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nilu</t>
+    <t xml:space="preserve">Propreitor’s Capital</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Investment Capital</t>
   </si>
   <si>
     <t xml:space="preserve">Current Assets</t>
@@ -43,12 +43,15 @@
     <t xml:space="preserve">Bank</t>
   </si>
   <si>
-    <t xml:space="preserve">xyz</t>
+    <t xml:space="preserve">SBI</t>
   </si>
   <si>
     <t xml:space="preserve">Cash</t>
   </si>
   <si>
+    <t xml:space="preserve">Cash In Hand</t>
+  </si>
+  <si>
     <t xml:space="preserve">Inventory</t>
   </si>
   <si>
@@ -64,18 +67,27 @@
     <t xml:space="preserve">Duties &amp; Taxes</t>
   </si>
   <si>
+    <t xml:space="preserve">SGSTIN_MH2.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CGSTIN_MH2.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IGSTIN_MH5.0</t>
+  </si>
+  <si>
     <t xml:space="preserve">Provisions</t>
   </si>
   <si>
-    <t xml:space="preserve">pqr</t>
-  </si>
-  <si>
     <t xml:space="preserve">Sundry Creditors for Expense</t>
   </si>
   <si>
     <t xml:space="preserve">Sundry Creditors for Purchase</t>
   </si>
   <si>
+    <t xml:space="preserve">Real Decors</t>
+  </si>
+  <si>
     <t xml:space="preserve">Direct Expense</t>
   </si>
   <si>
@@ -85,12 +97,18 @@
     <t xml:space="preserve">Purchase</t>
   </si>
   <si>
+    <t xml:space="preserve">Sponge Purchase</t>
+  </si>
+  <si>
     <t xml:space="preserve">Direct Income</t>
   </si>
   <si>
     <t xml:space="preserve">Sales</t>
   </si>
   <si>
+    <t xml:space="preserve">Sofa Sale</t>
+  </si>
+  <si>
     <t xml:space="preserve">Fixed Assets</t>
   </si>
   <si>
@@ -109,10 +127,13 @@
     <t xml:space="preserve">Indirect Expense</t>
   </si>
   <si>
+    <t xml:space="preserve">Electricity  Charges</t>
+  </si>
+  <si>
     <t xml:space="preserve">Indirect Income</t>
   </si>
   <si>
-    <t xml:space="preserve">kiuy</t>
+    <t xml:space="preserve">Sale of Old Laptops</t>
   </si>
   <si>
     <t xml:space="preserve">Investments</t>
@@ -150,7 +171,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.00"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="12">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -207,6 +228,20 @@
       <charset val="1"/>
     </font>
     <font>
+      <i val="true"/>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <i val="true"/>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="0"/>
@@ -255,7 +290,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -288,18 +323,26 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -309,10 +352,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C39"/>
+  <dimension ref="A1:C46"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A32" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A35" activeCellId="0" sqref="A35"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A37" activeCellId="0" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -379,61 +422,64 @@
       <c r="B8" s="3"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="5"/>
-    </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="3" t="n">
+        <v>300000</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="6" t="s">
         <v>10</v>
       </c>
+      <c r="C10" s="5"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="2" t="s">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B13" s="3"/>
-    </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C13" s="3"/>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="6" t="s">
         <v>14</v>
       </c>
+      <c r="B14" s="3"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="7" t="s">
         <v>15</v>
       </c>
       <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-    </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="6" t="s">
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="7" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="6" t="s">
+      <c r="B16" s="3"/>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="7" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="2" t="s">
+      <c r="B17" s="3"/>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="5"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="6" t="s">
@@ -445,20 +491,19 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="2" t="s">
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="3"/>
-    </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="7" t="s">
+    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B22" s="8"/>
+      <c r="C22" s="5"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="2" t="s">
+      <c r="A23" s="6" t="s">
         <v>23</v>
       </c>
     </row>
@@ -468,24 +513,27 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="6" t="s">
+      <c r="A25" s="7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="6" t="s">
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="2" t="s">
         <v>26</v>
       </c>
+      <c r="C26" s="3"/>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="6" t="s">
+      <c r="A27" s="8" t="s">
         <v>27</v>
       </c>
+      <c r="B27" s="9"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="2" t="s">
+      <c r="A28" s="10" t="s">
         <v>28</v>
       </c>
+      <c r="B28" s="9"/>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="s">
@@ -493,12 +541,12 @@
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="4" t="s">
+      <c r="A30" s="6" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="2" t="s">
+      <c r="A31" s="6" t="s">
         <v>31</v>
       </c>
     </row>
@@ -506,7 +554,6 @@
       <c r="A32" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C32" s="8"/>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="6" t="s">
@@ -519,17 +566,17 @@
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="2" t="s">
+      <c r="A35" s="10" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="6" t="s">
+      <c r="A36" s="2" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="6" t="s">
+      <c r="A37" s="4" t="s">
         <v>37</v>
       </c>
     </row>
@@ -539,8 +586,44 @@
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="2" t="s">
+      <c r="A39" s="6" t="s">
         <v>39</v>
+      </c>
+      <c r="C39" s="9"/>
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="2" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed balances of Capital Accounts
</commit_message>
<xml_diff>
--- a/gkwebapp/static/spreadsheets/Account_Import_Spreadsheet.xlsx
+++ b/gkwebapp/static/spreadsheets/Account_Import_Spreadsheet.xlsx
@@ -171,7 +171,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.00"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="13">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -220,6 +220,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+      <family val="0"/>
     </font>
     <font>
       <sz val="11"/>
@@ -290,7 +295,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -319,11 +324,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -331,7 +344,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -354,8 +367,8 @@
   </sheetPr>
   <dimension ref="A1:C46"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A37" activeCellId="0" sqref="A37"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -384,7 +397,8 @@
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="5" t="n">
+      <c r="B3" s="5"/>
+      <c r="C3" s="6" t="n">
         <v>144000</v>
       </c>
     </row>
@@ -392,7 +406,9 @@
       <c r="A4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="5"/>
+      <c r="C4" s="7" t="n">
+        <v>264000</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
@@ -402,7 +418,7 @@
       <c r="C5" s="5"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="8" t="s">
         <v>6</v>
       </c>
     </row>
@@ -416,13 +432,13 @@
       <c r="C7" s="3"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="8" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="3"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="9" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="3" t="n">
@@ -430,18 +446,18 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="8" t="s">
         <v>10</v>
       </c>
       <c r="C10" s="5"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="8" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="8" t="s">
         <v>12</v>
       </c>
     </row>
@@ -453,46 +469,46 @@
       <c r="C13" s="3"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="8" t="s">
         <v>14</v>
       </c>
       <c r="B14" s="3"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="9" t="s">
         <v>15</v>
       </c>
       <c r="B15" s="3"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="7" t="s">
+      <c r="A16" s="9" t="s">
         <v>16</v>
       </c>
       <c r="B16" s="3"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="7" t="s">
+      <c r="A17" s="9" t="s">
         <v>17</v>
       </c>
       <c r="B17" s="3"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="8" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="8" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="6" t="s">
+      <c r="A20" s="8" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="7" t="s">
+      <c r="A21" s="9" t="s">
         <v>21</v>
       </c>
     </row>
@@ -503,17 +519,17 @@
       <c r="C22" s="5"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="6" t="s">
+      <c r="A23" s="8" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="6" t="s">
+      <c r="A24" s="8" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="7" t="s">
+      <c r="A25" s="9" t="s">
         <v>25</v>
       </c>
     </row>
@@ -524,16 +540,16 @@
       <c r="C26" s="3"/>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="8" t="s">
+      <c r="A27" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="B27" s="9"/>
+      <c r="B27" s="11"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="10" t="s">
+      <c r="A28" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="B28" s="9"/>
+      <c r="B28" s="11"/>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="s">
@@ -541,22 +557,22 @@
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="6" t="s">
+      <c r="A30" s="8" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="6" t="s">
+      <c r="A31" s="8" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="6" t="s">
+      <c r="A32" s="8" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="6" t="s">
+      <c r="A33" s="8" t="s">
         <v>33</v>
       </c>
     </row>
@@ -566,7 +582,7 @@
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="10" t="s">
+      <c r="A35" s="12" t="s">
         <v>35</v>
       </c>
     </row>
@@ -586,13 +602,13 @@
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="6" t="s">
+      <c r="A39" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="C39" s="9"/>
+      <c r="C39" s="11"/>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="6" t="s">
+      <c r="A40" s="8" t="s">
         <v>40</v>
       </c>
     </row>
@@ -607,12 +623,12 @@
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="6" t="s">
+      <c r="A43" s="8" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="6" t="s">
+      <c r="A44" s="8" t="s">
         <v>44</v>
       </c>
     </row>

</xml_diff>